<commit_message>
Fixing map and mario sprite draw so ugly. Include tited tmx
</commit_message>
<xml_diff>
--- a/MarioBros/Data/Mario_Sprite_Info.xlsx
+++ b/MarioBros/Data/Mario_Sprite_Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sku\MarioSE\MarioBros\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D21DEC4-076B-45D2-828D-C1EB28FD8964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11D5546-5BA1-407F-9386-10D9211A8CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4008" yWindow="4380" windowWidth="23040" windowHeight="13560" xr2:uid="{867B155F-DB01-4004-9399-083B90F548E1}"/>
   </bookViews>
@@ -563,16 +563,16 @@
         <v>11121</v>
       </c>
       <c r="B59">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C59">
         <v>154</v>
       </c>
       <c r="D59">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E59">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -583,16 +583,16 @@
         <v>11111</v>
       </c>
       <c r="B60">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C60">
         <v>154</v>
       </c>
       <c r="D60">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E60">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -608,7 +608,7 @@
         <v>11222</v>
       </c>
       <c r="B63">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C63">
         <v>154</v>
@@ -617,7 +617,7 @@
         <v>290</v>
       </c>
       <c r="E63">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -628,7 +628,7 @@
         <v>11223</v>
       </c>
       <c r="B64">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C64">
         <v>154</v>
@@ -637,7 +637,7 @@
         <v>321</v>
       </c>
       <c r="E64">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -653,7 +653,7 @@
         <v>11212</v>
       </c>
       <c r="B67">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C67">
         <v>154</v>
@@ -662,7 +662,7 @@
         <v>170</v>
       </c>
       <c r="E67">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -673,7 +673,7 @@
         <v>11213</v>
       </c>
       <c r="B68">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C68">
         <v>154</v>
@@ -682,7 +682,7 @@
         <v>140</v>
       </c>
       <c r="E68">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -698,7 +698,7 @@
         <v>11321</v>
       </c>
       <c r="B71">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C71">
         <v>154</v>
@@ -707,7 +707,7 @@
         <v>355</v>
       </c>
       <c r="E71">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -718,7 +718,7 @@
         <v>11322</v>
       </c>
       <c r="B72">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C72">
         <v>154</v>
@@ -727,7 +727,7 @@
         <v>355</v>
       </c>
       <c r="E72">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -738,7 +738,7 @@
         <v>11323</v>
       </c>
       <c r="B73">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C73">
         <v>154</v>
@@ -747,7 +747,7 @@
         <v>413</v>
       </c>
       <c r="E73">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -763,7 +763,7 @@
         <v>11311</v>
       </c>
       <c r="B76">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C76">
         <v>154</v>
@@ -772,7 +772,7 @@
         <v>112</v>
       </c>
       <c r="E76">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -783,7 +783,7 @@
         <v>11312</v>
       </c>
       <c r="B77">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C77">
         <v>154</v>
@@ -792,7 +792,7 @@
         <v>86</v>
       </c>
       <c r="E77">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -803,7 +803,7 @@
         <v>11313</v>
       </c>
       <c r="B78">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C78">
         <v>154</v>
@@ -812,7 +812,7 @@
         <v>55</v>
       </c>
       <c r="E78">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -828,7 +828,7 @@
         <v>11417</v>
       </c>
       <c r="B81">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C81">
         <v>275</v>
@@ -848,7 +848,7 @@
         <v>11413</v>
       </c>
       <c r="B82">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C82">
         <v>275</v>
@@ -879,10 +879,10 @@
         <v>195</v>
       </c>
       <c r="D85">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E85">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F85">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>11423</v>
       </c>
       <c r="B86">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C86">
         <v>195</v>
@@ -902,7 +902,7 @@
         <v>52</v>
       </c>
       <c r="E86">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F86">
         <v>0</v>
@@ -963,7 +963,7 @@
         <v>11621</v>
       </c>
       <c r="B93">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C93">
         <v>154</v>
@@ -972,7 +972,7 @@
         <v>442</v>
       </c>
       <c r="E93">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F93">
         <v>0</v>
@@ -983,7 +983,7 @@
         <v>11611</v>
       </c>
       <c r="B94">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C94">
         <v>154</v>
@@ -992,7 +992,7 @@
         <v>22</v>
       </c>
       <c r="E94">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F94">
         <v>0</v>
@@ -1309,10 +1309,10 @@
         <v>0</v>
       </c>
       <c r="D123">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E123">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F123">
         <v>0</v>
@@ -1329,10 +1329,10 @@
         <v>0</v>
       </c>
       <c r="D124">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E124">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F124">
         <v>0</v>
@@ -1348,7 +1348,7 @@
         <v>12413</v>
       </c>
       <c r="B127">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C127">
         <v>80</v>
@@ -1357,7 +1357,7 @@
         <v>50</v>
       </c>
       <c r="E127">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F127">
         <v>0</v>
@@ -1368,7 +1368,7 @@
         <v>12417</v>
       </c>
       <c r="B128">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C128">
         <v>80</v>
@@ -1377,7 +1377,7 @@
         <v>410</v>
       </c>
       <c r="E128">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F128">
         <v>0</v>
@@ -1393,7 +1393,7 @@
         <v>12423</v>
       </c>
       <c r="B131">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C131">
         <v>40</v>
@@ -1402,7 +1402,7 @@
         <v>80</v>
       </c>
       <c r="E131">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F131">
         <v>0</v>
@@ -1413,7 +1413,7 @@
         <v>12427</v>
       </c>
       <c r="B132">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C132">
         <v>40</v>
@@ -1422,7 +1422,7 @@
         <v>380</v>
       </c>
       <c r="E132">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F132">
         <v>0</v>

</xml_diff>